<commit_message>
logging added to exact method same depth test everywhere in visibility check
</commit_message>
<xml_diff>
--- a/Plucker.xlsx
+++ b/Plucker.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PhD\PluckerCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC20FC33-781A-4750-B064-68E3089818B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB85DF39-E109-4EEA-8BB4-30B6D8A0ADF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15000" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FFD39C26-6585-4609-B32E-4907BCA2A0AC}"/>
+    <workbookView xWindow="-15000" yWindow="16080" windowWidth="29040" windowHeight="15840" xr2:uid="{FFD39C26-6585-4609-B32E-4907BCA2A0AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="39">
   <si>
     <t>alldir = false</t>
   </si>
@@ -132,6 +133,24 @@
   </si>
   <si>
     <t>Completed RST1 in 29912 ms</t>
+  </si>
+  <si>
+    <t>Combi Cache, Size: 837158 Hits: 4642622 Hash Hit Size: 0</t>
+  </si>
+  <si>
+    <t>Edge Edge Edge Cache, Size: 3101 Hits: 53860</t>
+  </si>
+  <si>
+    <t>Edge Edge Cache, Size: 1196 Hits: 21812</t>
+  </si>
+  <si>
+    <t>Completed RST1 in 16481 ms</t>
+  </si>
+  <si>
+    <t>cacheEE = true</t>
+  </si>
+  <si>
+    <t>cacheEEE = true</t>
   </si>
 </sst>
 </file>
@@ -485,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EBC88E0-7ADB-41FA-A749-8B6A7ABA762C}">
   <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,15 +612,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1838DC1-A8D6-48E8-95A2-AF9E6F042AB5}">
-  <dimension ref="A1:AA22"/>
+  <dimension ref="A1:AF23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W23" sqref="W23"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AF33" sqref="AF33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -617,8 +636,11 @@
       <c r="AA1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -634,8 +656,11 @@
       <c r="AA2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -651,8 +676,11 @@
       <c r="AA3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -668,8 +696,11 @@
       <c r="AA4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -685,8 +716,11 @@
       <c r="AA5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -702,8 +736,11 @@
       <c r="AA6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -719,8 +756,11 @@
       <c r="AA7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -736,8 +776,11 @@
       <c r="AA8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -753,8 +796,11 @@
       <c r="AA9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -770,8 +816,11 @@
       <c r="AA10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -787,8 +836,11 @@
       <c r="AA11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -804,8 +856,11 @@
       <c r="AA12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -821,8 +876,11 @@
       <c r="AA13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -838,8 +896,11 @@
       <c r="AA14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -855,8 +916,11 @@
       <c r="AA15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -872,8 +936,11 @@
       <c r="AA16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -889,8 +956,11 @@
       <c r="AA17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -906,8 +976,11 @@
       <c r="AA18" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -917,8 +990,11 @@
       <c r="U20" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -934,10 +1010,21 @@
       <c r="AA21" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="N22" t="s">
         <v>28</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AF23" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>